<commit_message>
Update documentation and planification, and add design files
</commit_message>
<xml_diff>
--- a/Documentation/FBN_journal_travail.xlsx
+++ b/Documentation/FBN_journal_travail.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="47">
   <si>
     <t>Date</t>
   </si>
@@ -156,6 +156,24 @@
   </si>
   <si>
     <t>Création carrefours (les feux)</t>
+  </si>
+  <si>
+    <t>Après disscussion avec le chef de projet, il a été convenu que le type des véhicules seront aléatoires</t>
+  </si>
+  <si>
+    <t>Suite de la création des carrefours (les feux)</t>
+  </si>
+  <si>
+    <t>Création des carrefours (les giratoires)</t>
+  </si>
+  <si>
+    <t>Création des voitures</t>
+  </si>
+  <si>
+    <t>Mise en place du serveur web</t>
+  </si>
+  <si>
+    <t>Création des motos</t>
   </si>
 </sst>
 </file>
@@ -677,8 +695,8 @@
         <v>2</v>
       </c>
       <c r="B1" s="15">
-        <f>Journal!B20</f>
-        <v>0.71875</v>
+        <f>Journal!B25</f>
+        <v>0.9375</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="21" x14ac:dyDescent="0.25">
@@ -686,7 +704,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="17">
-        <f>Journal!B23</f>
+        <f>Journal!B28</f>
         <v>0</v>
       </c>
     </row>
@@ -695,7 +713,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="19">
-        <f>Journal!B26</f>
+        <f>Journal!B31</f>
         <v>0</v>
       </c>
     </row>
@@ -704,7 +722,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="21">
-        <f>Journal!B29</f>
+        <f>Journal!B34</f>
         <v>0</v>
       </c>
     </row>
@@ -713,7 +731,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="25">
-        <f>Journal!B32</f>
+        <f>Journal!B37</f>
         <v>0</v>
       </c>
     </row>
@@ -723,7 +741,7 @@
       </c>
       <c r="B6" s="23">
         <f>SUM(B1:B5)</f>
-        <v>0.71875</v>
+        <v>0.9375</v>
       </c>
     </row>
   </sheetData>
@@ -737,10 +755,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -805,7 +823,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" s="8" customFormat="1" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>43592</v>
       </c>
@@ -974,12 +992,12 @@
       </c>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" s="8" customFormat="1" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>43594</v>
       </c>
       <c r="B16" s="11">
-        <v>8.3333333333333329E-2</v>
+        <v>0.10416666666666667</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>36</v>
@@ -987,7 +1005,9 @@
       <c r="D16" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E16" s="2"/>
+      <c r="E16" s="2" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="17" spans="1:5" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
@@ -1009,7 +1029,7 @@
         <v>43594</v>
       </c>
       <c r="B18" s="11">
-        <v>7.2916666666666671E-2</v>
+        <v>5.2083333333333336E-2</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>36</v>
@@ -1020,148 +1040,188 @@
       <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="13"/>
+      <c r="A19" s="7">
+        <v>43595</v>
+      </c>
+      <c r="B19" s="11">
+        <v>3.125E-2</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>42</v>
+      </c>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+    <row r="20" spans="1:5" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="7">
+        <v>43595</v>
+      </c>
+      <c r="B20" s="11">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:5" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="7">
+        <v>43595</v>
+      </c>
+      <c r="B21" s="11">
+        <v>0.125</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="1:5" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="7">
+        <v>43595</v>
+      </c>
+      <c r="B22" s="11">
+        <v>3.125E-2</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="1:5" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="7">
+        <v>43595</v>
+      </c>
+      <c r="B23" s="11">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="1:5" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="7"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="2"/>
+    </row>
+    <row r="25" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="10">
-        <f>SUM(B4:B19)</f>
-        <v>0.71875</v>
-      </c>
-      <c r="D20" s="12"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="26" t="s">
+      <c r="B25" s="10">
+        <f>SUM(B4:B24)</f>
+        <v>0.9375</v>
+      </c>
+      <c r="D25" s="12"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="26"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
-    </row>
-    <row r="22" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="10"/>
-      <c r="D22" s="12"/>
-    </row>
-    <row r="23" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
+    </row>
+    <row r="27" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="10"/>
+      <c r="D27" s="12"/>
+    </row>
+    <row r="28" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="10">
-        <f>SUM(B22:B22)</f>
+      <c r="B28" s="10">
+        <f>SUM(B27:B27)</f>
         <v>0</v>
       </c>
-      <c r="D23" s="12"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="26" t="s">
+      <c r="D28" s="12"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="B24" s="26"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26"/>
-    </row>
-    <row r="25" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="10"/>
-      <c r="D25" s="12"/>
-    </row>
-    <row r="26" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+    </row>
+    <row r="30" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="10"/>
+      <c r="D30" s="12"/>
+    </row>
+    <row r="31" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B26" s="10">
-        <f>SUM(B25:B25)</f>
+      <c r="B31" s="10">
+        <f>SUM(B30:B30)</f>
         <v>0</v>
       </c>
-      <c r="D26" s="12"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="26" t="s">
+      <c r="D31" s="12"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="B27" s="26"/>
-      <c r="C27" s="26"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="26"/>
-    </row>
-    <row r="28" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="10"/>
-      <c r="D28" s="12"/>
-    </row>
-    <row r="29" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
+      <c r="B32" s="26"/>
+      <c r="C32" s="26"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="26"/>
+    </row>
+    <row r="33" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="10"/>
+      <c r="D33" s="12"/>
+    </row>
+    <row r="34" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B29" s="10">
-        <f>SUM(B28:B28)</f>
+      <c r="B34" s="10">
+        <f>SUM(B33:B33)</f>
         <v>0</v>
       </c>
-      <c r="D29" s="12"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="26" t="s">
+      <c r="D34" s="12"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="26"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
-    </row>
-    <row r="31" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="10"/>
-      <c r="D31" s="12"/>
-    </row>
-    <row r="32" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
+      <c r="B35" s="26"/>
+      <c r="C35" s="26"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="26"/>
+    </row>
+    <row r="36" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="10"/>
+      <c r="D36" s="12"/>
+    </row>
+    <row r="37" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B32" s="10">
-        <f>SUM(B31:B31)</f>
+      <c r="B37" s="10">
+        <f>SUM(B36:B36)</f>
         <v>0</v>
       </c>
-      <c r="D32" s="12"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="5"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="5"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="5"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="5"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="5"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
+      <c r="D37" s="12"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
@@ -1170,14 +1230,49 @@
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
     </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="5"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="5"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="5"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="5"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="5"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
+    </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A30:E30"/>
+    <mergeCell ref="A35:E35"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A21:E21"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="A27:E27"/>
+    <mergeCell ref="A26:E26"/>
+    <mergeCell ref="A29:E29"/>
+    <mergeCell ref="A32:E32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" scale="92" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>